<commit_message>
Cambio de nombre por nomenclatura incorrecta
</commit_message>
<xml_diff>
--- a/Proyectos/ControlDeGastos/02. Planeación/ControlDeGastos-PlanProyecto.xlsx
+++ b/Proyectos/ControlDeGastos/02. Planeación/ControlDeGastos-PlanProyecto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Generales" sheetId="1" state="visible" r:id="rId2"/>
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="153">
   <si>
     <t>Plan de Proyecto</t>
   </si>
@@ -196,7 +196,7 @@
     <t>Empresa:</t>
   </si>
   <si>
-    <t>&lt;Nombre de la Empresa Cliente&gt;</t>
+    <t>Qualtop</t>
   </si>
   <si>
     <t>Emitido por: </t>
@@ -208,9 +208,6 @@
     <t>Fecha de Emisión:</t>
   </si>
   <si>
-    <t>&lt;Fecha&gt;</t>
-  </si>
-  <si>
     <t>Estrategia</t>
   </si>
   <si>
@@ -247,22 +244,13 @@
     <t>Objetivos de Calidad</t>
   </si>
   <si>
-    <t>Presentacion de proyecto</t>
-  </si>
-  <si>
-    <t>Mostrar al cliente equipo de trabajo y metodologia para realizar el proyecto del cliente</t>
-  </si>
-  <si>
-    <t>instalador</t>
-  </si>
-  <si>
-    <t>Ejecutable de programa que instala el producto solicitado por el cliente en diversas maquinas</t>
-  </si>
-  <si>
-    <t>Manual de usuario</t>
-  </si>
-  <si>
-    <t>Manual para ayudar al usuario a dar uso sobre el sistema</t>
+    <t>Manual de Usuario</t>
+  </si>
+  <si>
+    <t>Validar la correcta transacción de sistema al cliente con su correcto funcionamiento</t>
+  </si>
+  <si>
+    <t>Software Implementado</t>
   </si>
   <si>
     <t>Hitos del Proyecto</t>
@@ -373,19 +361,19 @@
     <t>Fecha Real</t>
   </si>
   <si>
-    <t>Github</t>
-  </si>
-  <si>
-    <t>Mayra Tejeda,Vianey Castillo,Ignacio Martinez</t>
-  </si>
-  <si>
-    <t>Source Tree</t>
-  </si>
-  <si>
-    <t>Toggl</t>
-  </si>
-  <si>
-    <t>Equipo del &lt;Cliente&gt;</t>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Equipo del Qualtop</t>
+  </si>
+  <si>
+    <t>Rene Pulido</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>rpulido@qualtop.com</t>
   </si>
   <si>
     <t>Plan de Comunicación</t>
@@ -424,7 +412,13 @@
     <t>Resultados de monitoreo</t>
   </si>
   <si>
+    <t>Anayeli </t>
+  </si>
+  <si>
     <t>Presentar estado de monitoreo a dirección</t>
+  </si>
+  <si>
+    <t>Quincenal</t>
   </si>
   <si>
     <t>Finalización de codificación</t>
@@ -653,8 +647,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -1368,7 +1363,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="161">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1413,6 +1408,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1453,6 +1452,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1625,6 +1628,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1825,10 +1832,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="29" fillId="8" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1910,6 +1913,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2079,15 +2086,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1413000</xdr:colOff>
+      <xdr:colOff>1467000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3910680</xdr:colOff>
+      <xdr:colOff>3963960</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2100,8 +2107,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4194720" y="1080"/>
-          <a:ext cx="2497680" cy="823320"/>
+          <a:off x="4248720" y="1080"/>
+          <a:ext cx="2496960" cy="822600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2121,15 +2128,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>432000</xdr:colOff>
+      <xdr:colOff>486000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>154800</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>432360</xdr:colOff>
+      <xdr:colOff>486360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2138,7 +2145,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8243640" y="1011960"/>
+          <a:off x="8297640" y="993960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2164,15 +2171,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>927000</xdr:colOff>
+      <xdr:colOff>981000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>136080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>105480</xdr:colOff>
+      <xdr:colOff>158760</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>136440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2181,8 +2188,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4991400" y="1011240"/>
-          <a:ext cx="6349680" cy="360"/>
+          <a:off x="5045400" y="993240"/>
+          <a:ext cx="6348960" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2204,15 +2211,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>432000</xdr:colOff>
+      <xdr:colOff>486000</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>281880</xdr:rowOff>
+      <xdr:rowOff>263880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>432360</xdr:colOff>
+      <xdr:colOff>486360</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>282240</xdr:rowOff>
+      <xdr:rowOff>264240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2221,7 +2228,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8243640" y="5031000"/>
+          <a:off x="8297640" y="5013000"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2247,15 +2254,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>927000</xdr:colOff>
+      <xdr:colOff>981000</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>281880</xdr:rowOff>
+      <xdr:rowOff>263880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>105480</xdr:colOff>
+      <xdr:colOff>158760</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>282240</xdr:rowOff>
+      <xdr:rowOff>264240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2264,8 +2271,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4991400" y="5031000"/>
-          <a:ext cx="6349680" cy="360"/>
+          <a:off x="5045400" y="5013000"/>
+          <a:ext cx="6348960" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2287,15 +2294,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>135000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>47160</xdr:rowOff>
+      <xdr:rowOff>29160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>81360</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>13320</xdr:rowOff>
+      <xdr:colOff>135360</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>851760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2308,8 +2315,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12332520" y="47160"/>
-          <a:ext cx="360" cy="823320"/>
+          <a:off x="12386520" y="29160"/>
+          <a:ext cx="360" cy="822600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2329,15 +2336,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>574560</xdr:colOff>
+      <xdr:colOff>628560</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>40320</xdr:rowOff>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1633680</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:colOff>1686960</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>844920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2350,8 +2357,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10228320" y="40320"/>
-          <a:ext cx="2977560" cy="823320"/>
+          <a:off x="10282320" y="22320"/>
+          <a:ext cx="2976840" cy="822600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2371,15 +2378,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>746280</xdr:colOff>
+      <xdr:colOff>800280</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2120040</xdr:colOff>
+      <xdr:colOff>2173320</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>823320</xdr:rowOff>
+      <xdr:rowOff>822600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2392,8 +2399,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8222040" y="0"/>
-          <a:ext cx="2872440" cy="823320"/>
+          <a:off x="8276040" y="0"/>
+          <a:ext cx="2871720" cy="822600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2413,15 +2420,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1659600</xdr:colOff>
+      <xdr:colOff>1713600</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1834920</xdr:colOff>
+      <xdr:colOff>1888200</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>823320</xdr:rowOff>
+      <xdr:rowOff>822600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2434,8 +2441,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15034320" y="0"/>
-          <a:ext cx="3274200" cy="823320"/>
+          <a:off x="15088320" y="0"/>
+          <a:ext cx="3273480" cy="822600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2457,8 +2464,8 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2523,12 +2530,12 @@
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
+      <c r="C7" s="11" t="n">
+        <v>42466</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -2541,147 +2548,155 @@
       <c r="G8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="11"/>
+        <v>8</v>
+      </c>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="E10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="F10" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>14</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="5" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="15"/>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12"/>
+      <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="14"/>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11"/>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" s="16" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="11"/>
-    </row>
-    <row r="15" s="15" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="16" t="s">
+      <c r="C15" s="18" t="s">
         <v>19</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="5" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>24</v>
+      <c r="C17" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>26</v>
-      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="20"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="20"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="20"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
     </row>
     <row r="22" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="20"/>
-      <c r="B23" s="16" t="s">
+      <c r="A23" s="21"/>
+      <c r="B23" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="21"/>
+      <c r="B24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="22" t="n">
+        <v>42465</v>
+      </c>
+      <c r="D24" s="22" t="n">
+        <v>42465</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="21"/>
+      <c r="B25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C25" s="22" t="n">
+        <v>42471</v>
+      </c>
+      <c r="D25" s="22" t="n">
+        <v>42471</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="21"/>
+      <c r="B26" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="C26" s="22" t="n">
+        <v>42494</v>
+      </c>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="21"/>
+      <c r="B27" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="20"/>
-      <c r="B24" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="20"/>
-      <c r="B25" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20"/>
-      <c r="B26" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20"/>
-      <c r="B27" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="4"/>
+      <c r="C27" s="22" t="n">
+        <v>42501</v>
+      </c>
       <c r="D27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2690,38 +2705,38 @@
       <c r="D28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="21"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="C30" s="12"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="22"/>
+      <c r="B31" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="24"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
     </row>
     <row r="33" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="11"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="11"/>
+        <v>33</v>
+      </c>
+      <c r="C33" s="12"/>
     </row>
     <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="22"/>
+      <c r="B34" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2749,8 +2764,8 @@
   </sheetPr>
   <dimension ref="1:29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2788,257 +2803,253 @@
     <row r="1" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" s="26" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="27" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" s="24" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="25" t="s">
+      <c r="F4" s="27"/>
+      <c r="AMJ4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B5" s="28"/>
+      <c r="C5" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+    </row>
+    <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="31"/>
+      <c r="B6" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D6" s="30"/>
+      <c r="E6" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="F6" s="32"/>
+    </row>
+    <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="31"/>
+      <c r="B7" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="AMJ4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="26"/>
-      <c r="C5" s="27" t="s">
+      <c r="D7" s="30"/>
+      <c r="E7" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="32"/>
+    </row>
+    <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="31"/>
+      <c r="B8" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-    </row>
-    <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="29"/>
-      <c r="B6" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="27" t="s">
+      <c r="C8" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="30" t="s">
+      <c r="D8" s="30"/>
+      <c r="E8" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="30"/>
-    </row>
-    <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="29"/>
-      <c r="B7" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="27" t="s">
+      <c r="F8" s="28"/>
+    </row>
+    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="31"/>
+      <c r="B9" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="30"/>
-    </row>
-    <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29"/>
-      <c r="B8" s="26" t="s">
+      <c r="C9" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="D9" s="30"/>
+      <c r="E9" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="31" t="s">
+      <c r="F9" s="28"/>
+    </row>
+    <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="31"/>
+      <c r="B10" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="26"/>
-    </row>
-    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29"/>
-      <c r="B9" s="26" t="s">
+      <c r="C10" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="D10" s="30"/>
+      <c r="E10" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="31" t="s">
+      <c r="F10" s="28"/>
+    </row>
+    <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="31"/>
+      <c r="B11" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="26"/>
-    </row>
-    <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="29"/>
-      <c r="B10" s="26" t="s">
+      <c r="D11" s="30"/>
+      <c r="E11" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="28"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+    </row>
+    <row r="13" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B13" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="27" t="s">
+    </row>
+    <row r="14" s="26" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="31" t="s">
+      <c r="C14" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="26"/>
-    </row>
-    <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="29"/>
-      <c r="B11" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="27" t="s">
+      <c r="D14" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="26"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-    </row>
-    <row r="13" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="23" t="s">
+      <c r="E14" s="37" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" s="24" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="35" t="s">
+      <c r="AMJ14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="40"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="40"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="38"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40"/>
+    </row>
+    <row r="19" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+    </row>
+    <row r="20" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="35" t="s">
+    </row>
+    <row r="21" s="26" customFormat="true" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B21" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="27"/>
+      <c r="AMJ21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B22" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="C22" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="AMJ14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="36" t="s">
+      <c r="D22" s="30"/>
+      <c r="E22" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="38"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="37"/>
-      <c r="E16" s="38"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="37"/>
-      <c r="E17" s="38"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="38"/>
-    </row>
-    <row r="19" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-    </row>
-    <row r="20" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="40" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" s="24" customFormat="true" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="25"/>
-      <c r="AMJ21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="41"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
+      <c r="F22" s="32"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="41"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="41"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="41"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="41"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="41"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="41"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3080,6 +3091,7 @@
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1" display="zepeda.roque32@gmail.com"/>
     <hyperlink ref="E7" r:id="rId2" display="zepeda.roque32@gmail.com"/>
+    <hyperlink ref="E22" r:id="rId3" display="rpulido@qualtop.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3088,7 +3100,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -3099,8 +3111,8 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3161,243 +3173,249 @@
   <sheetData>
     <row r="1" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="43"/>
+      <c r="A2" s="45"/>
     </row>
     <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="44"/>
-      <c r="B3" s="45" t="s">
+      <c r="A3" s="46"/>
+      <c r="B3" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+    </row>
+    <row r="4" s="53" customFormat="true" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="49"/>
+      <c r="B4" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-    </row>
-    <row r="4" s="51" customFormat="true" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="47"/>
-      <c r="B4" s="48" t="s">
+      <c r="F4" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="G4" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="49" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="C5" s="55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="E5" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="G4" s="50" t="s">
+      <c r="F5" s="55" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="52" t="s">
+      <c r="G5" s="57"/>
+    </row>
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C6" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D6" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E6" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="F5" s="53" t="s">
+      <c r="F6" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="55"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="52" t="s">
+      <c r="G6" s="57"/>
+      <c r="L6" s="58"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C7" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="53" t="s">
+      <c r="E7" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="53"/>
-      <c r="G6" s="55"/>
-      <c r="L6" s="56"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="54"/>
-      <c r="E7" s="53" t="s">
-        <v>82</v>
-      </c>
-      <c r="F7" s="53" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" s="55"/>
-      <c r="L7" s="56"/>
+      <c r="F7" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="57"/>
+      <c r="L7" s="58"/>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="52"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="55"/>
-      <c r="L8" s="56"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="57"/>
+      <c r="L8" s="58"/>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="52"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="55"/>
-      <c r="L9" s="56"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="57"/>
+      <c r="L9" s="58"/>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="52"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="55"/>
-      <c r="L10" s="56"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="57"/>
+      <c r="L10" s="58"/>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="52"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="55"/>
-      <c r="L11" s="56"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="57"/>
+      <c r="L11" s="58"/>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="52"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="55"/>
-      <c r="L12" s="56"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="57"/>
+      <c r="L12" s="58"/>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="52"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="55"/>
-      <c r="L13" s="56"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="57"/>
+      <c r="L13" s="58"/>
     </row>
     <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="52"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="55"/>
-      <c r="L14" s="56"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="57"/>
+      <c r="L14" s="58"/>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="52"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="55"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="57"/>
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="52"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="55"/>
-      <c r="L16" s="56"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="57"/>
+      <c r="L16" s="58"/>
     </row>
     <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="52"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="55"/>
-      <c r="L17" s="56"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="57"/>
+      <c r="L17" s="58"/>
     </row>
     <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="52"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="55"/>
-      <c r="L18" s="56"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="57"/>
+      <c r="L18" s="58"/>
     </row>
     <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="52"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="55"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="57"/>
     </row>
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="52"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="55"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="57"/>
     </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="52"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="55"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="57"/>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="52"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="55"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="57"/>
     </row>
     <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="52"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="55"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="57"/>
     </row>
     <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="52"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="55"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="57"/>
     </row>
     <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="52"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="55"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="57"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -3426,7 +3444,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3442,186 +3460,206 @@
   <sheetData>
     <row r="1" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+    </row>
+    <row r="3" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-    </row>
-    <row r="3" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="59" t="s">
+      <c r="C3" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="D3" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="E3" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="F3" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="G3" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="F3" s="60" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="61" t="s">
+      <c r="B4" s="65" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="62" t="s">
+      <c r="C4" s="65"/>
+      <c r="D4" s="65" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" s="66" t="n">
+        <v>42488</v>
+      </c>
+      <c r="F4" s="66" t="n">
+        <v>42488</v>
+      </c>
+      <c r="G4" s="67"/>
+      <c r="J4" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="63" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63" t="n">
+      <c r="B5" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65" t="n">
         <v>5</v>
       </c>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="64"/>
-      <c r="J4" s="65" t="s">
+      <c r="E5" s="66" t="n">
+        <v>42488</v>
+      </c>
+      <c r="F5" s="66" t="n">
+        <v>42488</v>
+      </c>
+      <c r="G5" s="67"/>
+      <c r="J5" s="68" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="62" t="s">
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B6" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" s="66" t="n">
+        <v>42488</v>
+      </c>
+      <c r="F6" s="66" t="n">
+        <v>42488</v>
+      </c>
+      <c r="G6" s="67"/>
+      <c r="J6" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63" t="n">
-        <v>5</v>
-      </c>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="64"/>
-      <c r="J5" s="65" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="66" t="n">
+        <v>42488</v>
+      </c>
+      <c r="F7" s="66" t="n">
+        <v>42488</v>
+      </c>
+      <c r="G7" s="67"/>
+      <c r="J7" s="68"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="65" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="62" t="s">
-        <v>96</v>
-      </c>
-      <c r="B6" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63" t="n">
-        <v>5</v>
-      </c>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="64"/>
-      <c r="J6" s="65" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="62" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="64"/>
-      <c r="J7" s="65"/>
-    </row>
-    <row r="8" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="62" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="63" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63" t="n">
+      <c r="C8" s="65"/>
+      <c r="D8" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="64"/>
+      <c r="E8" s="66" t="n">
+        <v>42488</v>
+      </c>
+      <c r="F8" s="66" t="n">
+        <v>42488</v>
+      </c>
+      <c r="G8" s="67"/>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="62"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="64"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="67"/>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="62"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="64"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="67"/>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="62"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="64"/>
+      <c r="A11" s="64"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="67"/>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="62"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="64"/>
+      <c r="A12" s="64"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="67"/>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="62"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="64"/>
+      <c r="A13" s="64"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="67"/>
     </row>
     <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="62"/>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="64"/>
+      <c r="A14" s="64"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="67"/>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="62"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="64"/>
+      <c r="A15" s="64"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="67"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -3649,8 +3687,8 @@
   </sheetPr>
   <dimension ref="A1:IZ20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -3678,1002 +3716,1014 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="68.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="67"/>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="70"/>
-      <c r="IQ2" s="71" t="s">
+      <c r="A2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="73"/>
+      <c r="IQ2" s="74" t="s">
+        <v>98</v>
+      </c>
+      <c r="IR2" s="74"/>
+      <c r="IS2" s="74"/>
+      <c r="IT2" s="74"/>
+      <c r="IU2" s="74"/>
+      <c r="IV2" s="74"/>
+      <c r="IW2" s="74"/>
+      <c r="IX2" s="74"/>
+      <c r="IY2" s="74"/>
+      <c r="IZ2" s="74"/>
+    </row>
+    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="75" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="76"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="R3" s="80"/>
+      <c r="AD3" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="IR2" s="71"/>
-      <c r="IS2" s="71"/>
-      <c r="IT2" s="71"/>
-      <c r="IU2" s="71"/>
-      <c r="IV2" s="71"/>
-      <c r="IW2" s="71"/>
-      <c r="IX2" s="71"/>
-      <c r="IY2" s="71"/>
-      <c r="IZ2" s="71"/>
-    </row>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="72" t="s">
+      <c r="AE3" s="81" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
-      <c r="R3" s="77"/>
-      <c r="AD3" s="78" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="82" t="s">
         <v>102</v>
       </c>
-      <c r="AE3" s="78" t="s">
+      <c r="B4" s="82" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="79" t="s">
+      <c r="C4" s="83" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="D4" s="83" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="80" t="s">
+      <c r="E4" s="83" t="s">
         <v>106</v>
       </c>
-      <c r="D4" s="80" t="s">
+      <c r="F4" s="83" t="s">
         <v>107</v>
       </c>
-      <c r="E4" s="80" t="s">
+      <c r="G4" s="83" t="s">
         <v>108</v>
       </c>
-      <c r="F4" s="80" t="s">
+      <c r="H4" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="83" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="80" t="s">
+      <c r="J4" s="83" t="s">
         <v>110</v>
       </c>
-      <c r="H4" s="80" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" s="80" t="s">
+      <c r="L4" s="84" t="s">
+        <v>105</v>
+      </c>
+      <c r="M4" s="85" t="n">
+        <v>5</v>
+      </c>
+      <c r="N4" s="86" t="n">
+        <v>5</v>
+      </c>
+      <c r="O4" s="87" t="n">
+        <v>10</v>
+      </c>
+      <c r="P4" s="88" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="89" t="n">
+        <v>20</v>
+      </c>
+      <c r="R4" s="90" t="n">
+        <v>25</v>
+      </c>
+      <c r="S4" s="91"/>
+      <c r="T4" s="92" t="s">
         <v>111</v>
       </c>
-      <c r="J4" s="80" t="s">
+      <c r="U4" s="92"/>
+      <c r="AD4" s="81" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE4" s="81" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="51.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="93" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="94" t="s">
         <v>112</v>
       </c>
-      <c r="L4" s="81" t="s">
-        <v>107</v>
-      </c>
-      <c r="M4" s="82" t="n">
-        <v>5</v>
-      </c>
-      <c r="N4" s="83" t="n">
-        <v>5</v>
-      </c>
-      <c r="O4" s="84" t="n">
-        <v>10</v>
-      </c>
-      <c r="P4" s="85" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q4" s="86" t="n">
-        <v>20</v>
-      </c>
-      <c r="R4" s="87" t="n">
-        <v>25</v>
-      </c>
-      <c r="S4" s="88"/>
-      <c r="T4" s="89" t="s">
-        <v>113</v>
-      </c>
-      <c r="U4" s="89"/>
-      <c r="AD4" s="78" t="s">
-        <v>102</v>
-      </c>
-      <c r="AE4" s="78" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="51.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="90" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="91" t="s">
-        <v>114</v>
-      </c>
-      <c r="C5" s="92" t="n">
+      <c r="C5" s="95" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="92" t="n">
+      <c r="D5" s="95" t="n">
         <v>3</v>
       </c>
-      <c r="E5" s="92" t="n">
+      <c r="E5" s="95" t="n">
         <f aca="false">PRODUCT(C5:D5)</f>
         <v>9</v>
       </c>
-      <c r="F5" s="91" t="s">
+      <c r="F5" s="94" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="94" t="s">
+        <v>114</v>
+      </c>
+      <c r="H5" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="95" t="s">
         <v>115</v>
       </c>
-      <c r="G5" s="91" t="s">
+      <c r="J5" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L5" s="84"/>
+      <c r="M5" s="85" t="n">
+        <v>4</v>
+      </c>
+      <c r="N5" s="97" t="n">
+        <v>4</v>
+      </c>
+      <c r="O5" s="98" t="n">
+        <v>8</v>
+      </c>
+      <c r="P5" s="99" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="90" t="n">
+        <v>16</v>
+      </c>
+      <c r="R5" s="90" t="n">
+        <v>20</v>
+      </c>
+      <c r="S5" s="91"/>
+      <c r="T5" s="100" t="s">
         <v>116</v>
       </c>
-      <c r="H5" s="92" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="92" t="s">
+      <c r="U5" s="101" t="s">
+        <v>104</v>
+      </c>
+      <c r="IR5" s="102" t="s">
+        <v>105</v>
+      </c>
+      <c r="IS5" s="103" t="s">
         <v>117</v>
       </c>
-      <c r="J5" s="93"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="82" t="n">
-        <v>4</v>
-      </c>
-      <c r="N5" s="94" t="n">
-        <v>4</v>
-      </c>
-      <c r="O5" s="95" t="n">
-        <v>8</v>
-      </c>
-      <c r="P5" s="96" t="n">
-        <v>12</v>
-      </c>
-      <c r="Q5" s="87" t="n">
-        <v>16</v>
-      </c>
-      <c r="R5" s="87" t="n">
-        <v>20</v>
-      </c>
-      <c r="S5" s="88"/>
-      <c r="T5" s="97" t="s">
-        <v>118</v>
-      </c>
-      <c r="U5" s="98" t="s">
-        <v>106</v>
-      </c>
-      <c r="IR5" s="99" t="s">
-        <v>107</v>
-      </c>
-      <c r="IS5" s="100" t="s">
-        <v>119</v>
-      </c>
-      <c r="IT5" s="34" t="n">
+      <c r="IT5" s="36" t="n">
         <v>0.9</v>
       </c>
-      <c r="IU5" s="101" t="n">
+      <c r="IU5" s="104" t="n">
         <f aca="false">(IU10*IT5)</f>
         <v>0.9</v>
       </c>
-      <c r="IV5" s="101" t="n">
+      <c r="IV5" s="104" t="n">
         <f aca="false">(IV10*IT5)</f>
         <v>1.8</v>
       </c>
-      <c r="IW5" s="102" t="n">
+      <c r="IW5" s="105" t="n">
         <f aca="false">(IW10*IT5)</f>
         <v>2.7</v>
       </c>
-      <c r="IX5" s="76" t="n">
+      <c r="IX5" s="79" t="n">
         <f aca="false">(IX10*IT5)</f>
         <v>3.6</v>
       </c>
-      <c r="IY5" s="103" t="n">
+      <c r="IY5" s="106" t="n">
         <f aca="false">(IY10*IT5)</f>
         <v>4.5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="41.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="104" t="n">
+      <c r="A6" s="107" t="n">
         <f aca="false">A5+1</f>
         <v>2</v>
       </c>
-      <c r="B6" s="91" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="92" t="n">
+      <c r="B6" s="94" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="95" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="92" t="n">
+      <c r="D6" s="95" t="n">
         <v>3</v>
       </c>
-      <c r="E6" s="92" t="n">
+      <c r="E6" s="95" t="n">
         <f aca="false">PRODUCT(C6:D6)</f>
         <v>12</v>
       </c>
-      <c r="F6" s="91" t="s">
+      <c r="F6" s="94" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" s="94" t="s">
+        <v>120</v>
+      </c>
+      <c r="H6" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="95" t="s">
+        <v>115</v>
+      </c>
+      <c r="J6" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L6" s="84"/>
+      <c r="M6" s="85" t="n">
+        <v>3</v>
+      </c>
+      <c r="N6" s="108" t="n">
+        <v>3</v>
+      </c>
+      <c r="O6" s="109" t="n">
+        <v>6</v>
+      </c>
+      <c r="P6" s="87" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="90" t="n">
+        <v>12</v>
+      </c>
+      <c r="R6" s="90" t="n">
+        <v>15</v>
+      </c>
+      <c r="S6" s="91"/>
+      <c r="T6" s="110" t="n">
+        <v>1</v>
+      </c>
+      <c r="U6" s="111" t="s">
         <v>121</v>
       </c>
-      <c r="G6" s="91" t="s">
+      <c r="IR6" s="102"/>
+      <c r="IS6" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="H6" s="92" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="92" t="s">
-        <v>117</v>
-      </c>
-      <c r="J6" s="93"/>
-      <c r="L6" s="81"/>
-      <c r="M6" s="82" t="n">
-        <v>3</v>
-      </c>
-      <c r="N6" s="105" t="n">
-        <v>3</v>
-      </c>
-      <c r="O6" s="106" t="n">
-        <v>6</v>
-      </c>
-      <c r="P6" s="84" t="n">
-        <v>9</v>
-      </c>
-      <c r="Q6" s="87" t="n">
-        <v>12</v>
-      </c>
-      <c r="R6" s="87" t="n">
-        <v>15</v>
-      </c>
-      <c r="S6" s="88"/>
-      <c r="T6" s="107" t="n">
-        <v>1</v>
-      </c>
-      <c r="U6" s="108" t="s">
-        <v>123</v>
-      </c>
-      <c r="IR6" s="99"/>
-      <c r="IS6" s="100" t="s">
-        <v>124</v>
-      </c>
-      <c r="IT6" s="34" t="n">
+      <c r="IT6" s="36" t="n">
         <v>0.7</v>
       </c>
-      <c r="IU6" s="109" t="n">
+      <c r="IU6" s="112" t="n">
         <f aca="false">(IU10*IT6)</f>
         <v>0.7</v>
       </c>
-      <c r="IV6" s="76" t="n">
+      <c r="IV6" s="79" t="n">
         <f aca="false">(IV10*IT6)</f>
         <v>1.4</v>
       </c>
-      <c r="IW6" s="110" t="n">
+      <c r="IW6" s="113" t="n">
         <f aca="false">(IW10*IT6)</f>
         <v>2.1</v>
       </c>
-      <c r="IX6" s="111" t="n">
+      <c r="IX6" s="114" t="n">
         <f aca="false">(IX10*IT6)</f>
         <v>2.8</v>
       </c>
-      <c r="IY6" s="112" t="n">
+      <c r="IY6" s="115" t="n">
         <f aca="false">(IY10*IT6)</f>
         <v>3.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="104" t="n">
+      <c r="A7" s="107" t="n">
         <f aca="false">A6+1</f>
         <v>3</v>
       </c>
-      <c r="B7" s="91" t="s">
-        <v>125</v>
-      </c>
-      <c r="C7" s="92" t="n">
+      <c r="B7" s="94" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="95" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="92" t="n">
+      <c r="D7" s="95" t="n">
         <v>4</v>
       </c>
-      <c r="E7" s="113" t="n">
+      <c r="E7" s="116" t="n">
         <f aca="false">PRODUCT(C7:D7)</f>
         <v>8</v>
       </c>
-      <c r="F7" s="91" t="s">
+      <c r="F7" s="94" t="s">
+        <v>124</v>
+      </c>
+      <c r="G7" s="94" t="s">
+        <v>125</v>
+      </c>
+      <c r="H7" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="95" t="s">
+        <v>115</v>
+      </c>
+      <c r="J7" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L7" s="84"/>
+      <c r="M7" s="85" t="n">
+        <v>2</v>
+      </c>
+      <c r="N7" s="117" t="n">
+        <v>2</v>
+      </c>
+      <c r="O7" s="118" t="n">
+        <v>4</v>
+      </c>
+      <c r="P7" s="119" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="120" t="n">
+        <v>8</v>
+      </c>
+      <c r="R7" s="87" t="n">
+        <v>10</v>
+      </c>
+      <c r="S7" s="121"/>
+      <c r="T7" s="110" t="n">
+        <v>2</v>
+      </c>
+      <c r="U7" s="122" t="s">
         <v>126</v>
       </c>
-      <c r="G7" s="91" t="s">
+      <c r="IR7" s="102"/>
+      <c r="IS7" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="H7" s="92"/>
-      <c r="I7" s="92" t="s">
-        <v>117</v>
-      </c>
-      <c r="J7" s="114"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="82" t="n">
-        <v>2</v>
-      </c>
-      <c r="N7" s="115" t="n">
-        <v>2</v>
-      </c>
-      <c r="O7" s="116" t="n">
-        <v>4</v>
-      </c>
-      <c r="P7" s="117" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q7" s="118" t="n">
-        <v>8</v>
-      </c>
-      <c r="R7" s="84" t="n">
-        <v>10</v>
-      </c>
-      <c r="S7" s="119"/>
-      <c r="T7" s="107" t="n">
-        <v>2</v>
-      </c>
-      <c r="U7" s="120" t="s">
-        <v>128</v>
-      </c>
-      <c r="IR7" s="99"/>
-      <c r="IS7" s="100" t="s">
-        <v>129</v>
-      </c>
-      <c r="IT7" s="34" t="n">
+      <c r="IT7" s="36" t="n">
         <v>0.5</v>
       </c>
-      <c r="IU7" s="109" t="n">
+      <c r="IU7" s="112" t="n">
         <f aca="false">(IU10*IT7)</f>
         <v>0.5</v>
       </c>
-      <c r="IV7" s="111" t="n">
+      <c r="IV7" s="114" t="n">
         <f aca="false">(IV10*IT7)</f>
         <v>1</v>
       </c>
-      <c r="IW7" s="76" t="n">
+      <c r="IW7" s="79" t="n">
         <f aca="false">(IW10*IT7)</f>
         <v>1.5</v>
       </c>
-      <c r="IX7" s="76" t="n">
+      <c r="IX7" s="79" t="n">
         <f aca="false">(IX10*IT7)</f>
         <v>2</v>
       </c>
-      <c r="IY7" s="121" t="n">
+      <c r="IY7" s="123" t="n">
         <f aca="false">(IY10*IT7)</f>
         <v>2.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="43.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="104" t="n">
+      <c r="A8" s="107" t="n">
         <f aca="false">A7+1</f>
         <v>4</v>
       </c>
-      <c r="B8" s="91" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="92" t="n">
+      <c r="B8" s="94" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="95" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="92" t="n">
+      <c r="D8" s="95" t="n">
         <v>2</v>
       </c>
-      <c r="E8" s="113" t="n">
+      <c r="E8" s="116" t="n">
         <f aca="false">PRODUCT(C8:D8)</f>
         <v>10</v>
       </c>
-      <c r="F8" s="91" t="s">
+      <c r="F8" s="94" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" s="94" t="s">
+        <v>130</v>
+      </c>
+      <c r="H8" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="95" t="s">
+        <v>115</v>
+      </c>
+      <c r="J8" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" s="84"/>
+      <c r="M8" s="85" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" s="124" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" s="125" t="n">
+        <v>2</v>
+      </c>
+      <c r="P8" s="126" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="127" t="n">
+        <v>4</v>
+      </c>
+      <c r="R8" s="109" t="n">
+        <v>5</v>
+      </c>
+      <c r="S8" s="91"/>
+      <c r="T8" s="110" t="n">
+        <v>3</v>
+      </c>
+      <c r="U8" s="122" t="s">
         <v>131</v>
       </c>
-      <c r="G8" s="91" t="s">
+      <c r="IR8" s="102"/>
+      <c r="IS8" s="103" t="s">
         <v>132</v>
       </c>
-      <c r="H8" s="92" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="92" t="s">
-        <v>117</v>
-      </c>
-      <c r="J8" s="114"/>
-      <c r="L8" s="81"/>
-      <c r="M8" s="82" t="n">
-        <v>1</v>
-      </c>
-      <c r="N8" s="122" t="n">
-        <v>1</v>
-      </c>
-      <c r="O8" s="123" t="n">
-        <v>2</v>
-      </c>
-      <c r="P8" s="124" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q8" s="125" t="n">
-        <v>4</v>
-      </c>
-      <c r="R8" s="106" t="n">
-        <v>5</v>
-      </c>
-      <c r="S8" s="88"/>
-      <c r="T8" s="107" t="n">
-        <v>3</v>
-      </c>
-      <c r="U8" s="120" t="s">
-        <v>133</v>
-      </c>
-      <c r="IR8" s="99"/>
-      <c r="IS8" s="100" t="s">
-        <v>134</v>
-      </c>
-      <c r="IT8" s="34" t="n">
+      <c r="IT8" s="36" t="n">
         <v>0.3</v>
       </c>
-      <c r="IU8" s="126" t="n">
+      <c r="IU8" s="128" t="n">
         <f aca="false">(IU10*IT8)</f>
         <v>0.3</v>
       </c>
-      <c r="IV8" s="110" t="n">
+      <c r="IV8" s="113" t="n">
         <f aca="false">(IV10*IT8)</f>
         <v>0.6</v>
       </c>
-      <c r="IW8" s="76" t="n">
+      <c r="IW8" s="79" t="n">
         <f aca="false">(IW10*IT8)</f>
         <v>0.9</v>
       </c>
-      <c r="IX8" s="76" t="n">
+      <c r="IX8" s="79" t="n">
         <f aca="false">(IX10*IT8)</f>
         <v>1.2</v>
       </c>
-      <c r="IY8" s="112" t="n">
+      <c r="IY8" s="115" t="n">
         <f aca="false">(IY10*IT8)</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="49" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="104" t="n">
+      <c r="A9" s="107" t="n">
         <f aca="false">A8+1</f>
         <v>5</v>
       </c>
-      <c r="B9" s="91" t="s">
-        <v>135</v>
-      </c>
-      <c r="C9" s="92" t="n">
+      <c r="B9" s="94" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="95" t="n">
         <v>3</v>
       </c>
-      <c r="D9" s="92" t="n">
+      <c r="D9" s="95" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="113" t="n">
+      <c r="E9" s="116" t="n">
         <f aca="false">PRODUCT(C9:D9)</f>
         <v>3</v>
       </c>
-      <c r="F9" s="91" t="s">
+      <c r="F9" s="94" t="s">
+        <v>134</v>
+      </c>
+      <c r="G9" s="94" t="s">
+        <v>135</v>
+      </c>
+      <c r="H9" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="95" t="s">
+        <v>115</v>
+      </c>
+      <c r="J9" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L9" s="85"/>
+      <c r="M9" s="129"/>
+      <c r="N9" s="130" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" s="131" t="n">
+        <v>2</v>
+      </c>
+      <c r="P9" s="130" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="131" t="n">
+        <v>4</v>
+      </c>
+      <c r="R9" s="130" t="n">
+        <v>5</v>
+      </c>
+      <c r="S9" s="132"/>
+      <c r="T9" s="110" t="n">
+        <v>4</v>
+      </c>
+      <c r="U9" s="122" t="s">
         <v>136</v>
       </c>
-      <c r="G9" s="91" t="s">
-        <v>137</v>
-      </c>
-      <c r="H9" s="92" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="92" t="s">
-        <v>117</v>
-      </c>
-      <c r="J9" s="114"/>
-      <c r="L9" s="82"/>
-      <c r="M9" s="127"/>
-      <c r="N9" s="128" t="n">
-        <v>1</v>
-      </c>
-      <c r="O9" s="129" t="n">
-        <v>2</v>
-      </c>
-      <c r="P9" s="128" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q9" s="129" t="n">
-        <v>4</v>
-      </c>
-      <c r="R9" s="128" t="n">
-        <v>5</v>
-      </c>
-      <c r="S9" s="130"/>
-      <c r="T9" s="107" t="n">
-        <v>4</v>
-      </c>
-      <c r="U9" s="120" t="s">
-        <v>138</v>
-      </c>
-      <c r="IR9" s="99"/>
-      <c r="IS9" s="100" t="s">
-        <v>129</v>
-      </c>
-      <c r="IT9" s="131" t="n">
+      <c r="IR9" s="102"/>
+      <c r="IS9" s="103" t="s">
+        <v>127</v>
+      </c>
+      <c r="IT9" s="133" t="n">
         <v>0.1</v>
       </c>
-      <c r="IU9" s="111" t="n">
+      <c r="IU9" s="114" t="n">
         <f aca="false">(IU10*IT9)</f>
         <v>0.1</v>
       </c>
-      <c r="IV9" s="132" t="n">
+      <c r="IV9" s="134" t="n">
         <f aca="false">(IV10*IT9)</f>
         <v>0.2</v>
       </c>
-      <c r="IW9" s="133" t="n">
+      <c r="IW9" s="135" t="n">
         <f aca="false">(IW10*IU9)</f>
         <v>0.3</v>
       </c>
-      <c r="IX9" s="133" t="n">
+      <c r="IX9" s="135" t="n">
         <f aca="false">(IX10*IT9)</f>
         <v>0.4</v>
       </c>
-      <c r="IY9" s="134" t="n">
+      <c r="IY9" s="136" t="n">
         <f aca="false">(IY10*IT9)</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="104" t="n">
+      <c r="A10" s="107" t="n">
         <f aca="false">A9+1</f>
         <v>6</v>
       </c>
-      <c r="B10" s="91"/>
-      <c r="C10" s="92"/>
-      <c r="D10" s="92"/>
-      <c r="E10" s="113" t="n">
+      <c r="B10" s="94"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="116" t="n">
         <f aca="false">PRODUCT(C10:D10)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="135"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="113"/>
-      <c r="J10" s="114"/>
-      <c r="L10" s="82"/>
-      <c r="M10" s="127"/>
-      <c r="N10" s="136" t="s">
-        <v>106</v>
-      </c>
-      <c r="O10" s="136"/>
-      <c r="P10" s="136"/>
-      <c r="Q10" s="136"/>
-      <c r="R10" s="136"/>
-      <c r="S10" s="137"/>
-      <c r="T10" s="107" t="n">
+      <c r="F10" s="137"/>
+      <c r="G10" s="94"/>
+      <c r="H10" s="95"/>
+      <c r="I10" s="116"/>
+      <c r="J10" s="138"/>
+      <c r="L10" s="85"/>
+      <c r="M10" s="129"/>
+      <c r="N10" s="139" t="s">
+        <v>104</v>
+      </c>
+      <c r="O10" s="139"/>
+      <c r="P10" s="139"/>
+      <c r="Q10" s="139"/>
+      <c r="R10" s="139"/>
+      <c r="S10" s="140"/>
+      <c r="T10" s="110" t="n">
         <v>5</v>
       </c>
-      <c r="U10" s="120" t="s">
-        <v>139</v>
-      </c>
-      <c r="IR10" s="138"/>
-      <c r="IS10" s="76"/>
-      <c r="IT10" s="100"/>
-      <c r="IU10" s="34" t="n">
+      <c r="U10" s="122" t="s">
+        <v>137</v>
+      </c>
+      <c r="IR10" s="141"/>
+      <c r="IS10" s="79"/>
+      <c r="IT10" s="103"/>
+      <c r="IU10" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="IV10" s="34" t="n">
+      <c r="IV10" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="IW10" s="34" t="n">
+      <c r="IW10" s="36" t="n">
         <v>3</v>
       </c>
-      <c r="IX10" s="34" t="n">
+      <c r="IX10" s="36" t="n">
         <v>4</v>
       </c>
-      <c r="IY10" s="139" t="n">
+      <c r="IY10" s="142" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="104" t="n">
+      <c r="A11" s="107" t="n">
         <f aca="false">A10+1</f>
         <v>7</v>
       </c>
-      <c r="B11" s="91"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="113" t="n">
+      <c r="B11" s="94"/>
+      <c r="C11" s="95"/>
+      <c r="D11" s="95"/>
+      <c r="E11" s="116" t="n">
         <f aca="false">PRODUCT(C11:D11)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="135"/>
-      <c r="G11" s="91"/>
-      <c r="H11" s="92"/>
-      <c r="I11" s="113"/>
-      <c r="J11" s="114"/>
-      <c r="L11" s="140"/>
-      <c r="M11" s="137"/>
-      <c r="N11" s="140"/>
-      <c r="O11" s="137"/>
-      <c r="P11" s="137"/>
-      <c r="Q11" s="137"/>
-      <c r="R11" s="137"/>
-      <c r="S11" s="137"/>
-      <c r="T11" s="97" t="s">
-        <v>118</v>
-      </c>
-      <c r="U11" s="141" t="s">
-        <v>107</v>
-      </c>
-      <c r="IR11" s="138"/>
-      <c r="IS11" s="76"/>
-      <c r="IT11" s="76"/>
-      <c r="IU11" s="100" t="s">
-        <v>129</v>
-      </c>
-      <c r="IV11" s="100" t="s">
-        <v>134</v>
-      </c>
-      <c r="IW11" s="100" t="s">
-        <v>140</v>
-      </c>
-      <c r="IX11" s="100" t="s">
-        <v>124</v>
-      </c>
-      <c r="IY11" s="142" t="s">
-        <v>119</v>
+      <c r="F11" s="137"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="95"/>
+      <c r="I11" s="116"/>
+      <c r="J11" s="138"/>
+      <c r="L11" s="143"/>
+      <c r="M11" s="140"/>
+      <c r="N11" s="143"/>
+      <c r="O11" s="140"/>
+      <c r="P11" s="140"/>
+      <c r="Q11" s="140"/>
+      <c r="R11" s="140"/>
+      <c r="S11" s="140"/>
+      <c r="T11" s="100" t="s">
+        <v>116</v>
+      </c>
+      <c r="U11" s="144" t="s">
+        <v>105</v>
+      </c>
+      <c r="IR11" s="141"/>
+      <c r="IS11" s="79"/>
+      <c r="IT11" s="79"/>
+      <c r="IU11" s="103" t="s">
+        <v>127</v>
+      </c>
+      <c r="IV11" s="103" t="s">
+        <v>132</v>
+      </c>
+      <c r="IW11" s="103" t="s">
+        <v>138</v>
+      </c>
+      <c r="IX11" s="103" t="s">
+        <v>122</v>
+      </c>
+      <c r="IY11" s="145" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="104" t="n">
+      <c r="A12" s="107" t="n">
         <f aca="false">A11+1</f>
         <v>8</v>
       </c>
-      <c r="B12" s="91"/>
-      <c r="C12" s="92"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="113" t="n">
+      <c r="B12" s="94"/>
+      <c r="C12" s="95"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="116" t="n">
         <f aca="false">PRODUCT(C12:D12)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="135"/>
-      <c r="G12" s="91"/>
-      <c r="H12" s="92"/>
-      <c r="I12" s="113"/>
-      <c r="J12" s="114"/>
-      <c r="L12" s="140"/>
-      <c r="M12" s="137"/>
-      <c r="N12" s="137"/>
-      <c r="O12" s="137"/>
-      <c r="P12" s="137"/>
-      <c r="Q12" s="137"/>
-      <c r="R12" s="137"/>
-      <c r="S12" s="137"/>
-      <c r="T12" s="107" t="n">
+      <c r="F12" s="137"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="95"/>
+      <c r="I12" s="116"/>
+      <c r="J12" s="138"/>
+      <c r="L12" s="143"/>
+      <c r="M12" s="140"/>
+      <c r="N12" s="140"/>
+      <c r="O12" s="140"/>
+      <c r="P12" s="140"/>
+      <c r="Q12" s="140"/>
+      <c r="R12" s="140"/>
+      <c r="S12" s="140"/>
+      <c r="T12" s="110" t="n">
         <v>1</v>
       </c>
-      <c r="U12" s="143" t="s">
-        <v>141</v>
-      </c>
-      <c r="IR12" s="138"/>
-      <c r="IS12" s="76"/>
-      <c r="IT12" s="34"/>
-      <c r="IU12" s="144" t="s">
-        <v>106</v>
-      </c>
-      <c r="IV12" s="144"/>
-      <c r="IW12" s="144"/>
-      <c r="IX12" s="144"/>
-      <c r="IY12" s="144"/>
+      <c r="U12" s="146" t="s">
+        <v>139</v>
+      </c>
+      <c r="IR12" s="141"/>
+      <c r="IS12" s="79"/>
+      <c r="IT12" s="36"/>
+      <c r="IU12" s="147" t="s">
+        <v>104</v>
+      </c>
+      <c r="IV12" s="147"/>
+      <c r="IW12" s="147"/>
+      <c r="IX12" s="147"/>
+      <c r="IY12" s="147"/>
     </row>
     <row r="13" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="104" t="n">
+      <c r="A13" s="107" t="n">
         <f aca="false">A12+1</f>
         <v>9</v>
       </c>
-      <c r="B13" s="91"/>
-      <c r="C13" s="92"/>
-      <c r="D13" s="92"/>
-      <c r="E13" s="113" t="n">
+      <c r="B13" s="94"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="116" t="n">
         <f aca="false">PRODUCT(C13:D13)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="135"/>
-      <c r="G13" s="91"/>
-      <c r="H13" s="92"/>
-      <c r="I13" s="113"/>
-      <c r="J13" s="114"/>
-      <c r="L13" s="140"/>
-      <c r="M13" s="137"/>
-      <c r="N13" s="137"/>
-      <c r="O13" s="137"/>
-      <c r="P13" s="137"/>
-      <c r="Q13" s="137"/>
-      <c r="R13" s="137"/>
-      <c r="S13" s="137"/>
-      <c r="T13" s="107" t="n">
+      <c r="F13" s="137"/>
+      <c r="G13" s="94"/>
+      <c r="H13" s="95"/>
+      <c r="I13" s="116"/>
+      <c r="J13" s="138"/>
+      <c r="L13" s="143"/>
+      <c r="M13" s="140"/>
+      <c r="N13" s="140"/>
+      <c r="O13" s="140"/>
+      <c r="P13" s="140"/>
+      <c r="Q13" s="140"/>
+      <c r="R13" s="140"/>
+      <c r="S13" s="140"/>
+      <c r="T13" s="110" t="n">
         <v>2</v>
       </c>
-      <c r="U13" s="108" t="s">
-        <v>142</v>
-      </c>
-      <c r="IR13" s="138"/>
-      <c r="IS13" s="76"/>
-      <c r="IT13" s="76"/>
-      <c r="IU13" s="76"/>
-      <c r="IV13" s="76"/>
-      <c r="IW13" s="76"/>
-      <c r="IX13" s="76"/>
-      <c r="IY13" s="121"/>
+      <c r="U13" s="111" t="s">
+        <v>140</v>
+      </c>
+      <c r="IR13" s="141"/>
+      <c r="IS13" s="79"/>
+      <c r="IT13" s="79"/>
+      <c r="IU13" s="79"/>
+      <c r="IV13" s="79"/>
+      <c r="IW13" s="79"/>
+      <c r="IX13" s="79"/>
+      <c r="IY13" s="123"/>
     </row>
     <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="104" t="n">
+      <c r="A14" s="107" t="n">
         <f aca="false">A13+1</f>
         <v>10</v>
       </c>
-      <c r="B14" s="91"/>
-      <c r="C14" s="92"/>
-      <c r="D14" s="92"/>
-      <c r="E14" s="113" t="n">
+      <c r="B14" s="94"/>
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="116" t="n">
         <f aca="false">PRODUCT(C14:D14)</f>
         <v>0</v>
       </c>
-      <c r="F14" s="135"/>
-      <c r="G14" s="91"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="113"/>
-      <c r="J14" s="114"/>
-      <c r="L14" s="140"/>
-      <c r="M14" s="137"/>
-      <c r="N14" s="137"/>
-      <c r="O14" s="137"/>
-      <c r="P14" s="137"/>
-      <c r="Q14" s="137"/>
-      <c r="R14" s="137"/>
-      <c r="S14" s="137"/>
-      <c r="T14" s="107" t="n">
+      <c r="F14" s="137"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="95"/>
+      <c r="I14" s="116"/>
+      <c r="J14" s="138"/>
+      <c r="L14" s="143"/>
+      <c r="M14" s="140"/>
+      <c r="N14" s="140"/>
+      <c r="O14" s="140"/>
+      <c r="P14" s="140"/>
+      <c r="Q14" s="140"/>
+      <c r="R14" s="140"/>
+      <c r="S14" s="140"/>
+      <c r="T14" s="110" t="n">
         <v>3</v>
       </c>
-      <c r="U14" s="120" t="s">
-        <v>143</v>
-      </c>
-      <c r="IR14" s="138"/>
-      <c r="IS14" s="76"/>
-      <c r="IT14" s="33"/>
-      <c r="IU14" s="33"/>
-      <c r="IV14" s="33"/>
-      <c r="IW14" s="33"/>
-      <c r="IX14" s="33"/>
-      <c r="IY14" s="145"/>
+      <c r="U14" s="122" t="s">
+        <v>141</v>
+      </c>
+      <c r="IR14" s="141"/>
+      <c r="IS14" s="79"/>
+      <c r="IT14" s="35"/>
+      <c r="IU14" s="35"/>
+      <c r="IV14" s="35"/>
+      <c r="IW14" s="35"/>
+      <c r="IX14" s="35"/>
+      <c r="IY14" s="148"/>
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="104" t="n">
+      <c r="A15" s="107" t="n">
         <f aca="false">A14+1</f>
         <v>11</v>
       </c>
-      <c r="B15" s="91"/>
-      <c r="C15" s="92"/>
-      <c r="D15" s="92"/>
-      <c r="E15" s="113" t="n">
+      <c r="B15" s="94"/>
+      <c r="C15" s="95"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="116" t="n">
         <f aca="false">PRODUCT(C15:D15)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="135"/>
-      <c r="G15" s="91"/>
-      <c r="H15" s="92"/>
-      <c r="I15" s="113"/>
-      <c r="J15" s="114"/>
-      <c r="L15" s="146"/>
-      <c r="M15" s="137"/>
-      <c r="N15" s="137"/>
-      <c r="O15" s="137"/>
-      <c r="P15" s="137"/>
-      <c r="Q15" s="137"/>
-      <c r="R15" s="137"/>
-      <c r="S15" s="137"/>
-      <c r="T15" s="107" t="n">
+      <c r="F15" s="137"/>
+      <c r="G15" s="94"/>
+      <c r="H15" s="95"/>
+      <c r="I15" s="116"/>
+      <c r="J15" s="138"/>
+      <c r="L15" s="149"/>
+      <c r="M15" s="140"/>
+      <c r="N15" s="140"/>
+      <c r="O15" s="140"/>
+      <c r="P15" s="140"/>
+      <c r="Q15" s="140"/>
+      <c r="R15" s="140"/>
+      <c r="S15" s="140"/>
+      <c r="T15" s="110" t="n">
         <v>4</v>
       </c>
-      <c r="U15" s="120" t="s">
-        <v>144</v>
-      </c>
-      <c r="IR15" s="147" t="s">
-        <v>145</v>
-      </c>
-      <c r="IS15" s="147"/>
-      <c r="IT15" s="33"/>
-      <c r="IU15" s="33"/>
-      <c r="IV15" s="33"/>
-      <c r="IW15" s="33"/>
-      <c r="IX15" s="33"/>
-      <c r="IY15" s="145"/>
+      <c r="U15" s="122" t="s">
+        <v>142</v>
+      </c>
+      <c r="IR15" s="150" t="s">
+        <v>143</v>
+      </c>
+      <c r="IS15" s="150"/>
+      <c r="IT15" s="35"/>
+      <c r="IU15" s="35"/>
+      <c r="IV15" s="35"/>
+      <c r="IW15" s="35"/>
+      <c r="IX15" s="35"/>
+      <c r="IY15" s="148"/>
     </row>
     <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="104" t="n">
+      <c r="A16" s="107" t="n">
         <f aca="false">A15+1</f>
         <v>12</v>
       </c>
-      <c r="B16" s="91"/>
-      <c r="C16" s="92"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="113" t="n">
+      <c r="B16" s="94"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="116" t="n">
         <f aca="false">PRODUCT(C16:D16)</f>
         <v>0</v>
       </c>
-      <c r="F16" s="135"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="113"/>
-      <c r="J16" s="114"/>
-      <c r="L16" s="146"/>
-      <c r="M16" s="137"/>
-      <c r="N16" s="137"/>
-      <c r="O16" s="137"/>
-      <c r="P16" s="137"/>
-      <c r="Q16" s="137"/>
-      <c r="R16" s="137"/>
-      <c r="S16" s="137"/>
-      <c r="T16" s="107" t="n">
+      <c r="F16" s="137"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="95"/>
+      <c r="I16" s="116"/>
+      <c r="J16" s="138"/>
+      <c r="L16" s="149"/>
+      <c r="M16" s="140"/>
+      <c r="N16" s="140"/>
+      <c r="O16" s="140"/>
+      <c r="P16" s="140"/>
+      <c r="Q16" s="140"/>
+      <c r="R16" s="140"/>
+      <c r="S16" s="140"/>
+      <c r="T16" s="110" t="n">
         <v>5</v>
       </c>
-      <c r="U16" s="143" t="s">
+      <c r="U16" s="146" t="s">
+        <v>144</v>
+      </c>
+      <c r="IR16" s="141" t="s">
+        <v>145</v>
+      </c>
+      <c r="IS16" s="151"/>
+      <c r="IT16" s="35"/>
+      <c r="IU16" s="152" t="s">
         <v>146</v>
       </c>
-      <c r="IR16" s="138" t="s">
-        <v>147</v>
-      </c>
-      <c r="IS16" s="148"/>
-      <c r="IT16" s="33"/>
-      <c r="IU16" s="149" t="s">
-        <v>148</v>
-      </c>
-      <c r="IV16" s="149"/>
-      <c r="IW16" s="149"/>
-      <c r="IX16" s="149"/>
-      <c r="IY16" s="149"/>
+      <c r="IV16" s="152"/>
+      <c r="IW16" s="152"/>
+      <c r="IX16" s="152"/>
+      <c r="IY16" s="152"/>
     </row>
     <row r="17" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="104" t="n">
+      <c r="A17" s="107" t="n">
         <f aca="false">A16+1</f>
         <v>13</v>
       </c>
-      <c r="B17" s="91"/>
-      <c r="C17" s="92"/>
-      <c r="D17" s="92"/>
-      <c r="E17" s="113" t="n">
+      <c r="B17" s="94"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="116" t="n">
         <f aca="false">PRODUCT(C17:D17)</f>
         <v>0</v>
       </c>
-      <c r="F17" s="135"/>
-      <c r="G17" s="91"/>
-      <c r="H17" s="92"/>
-      <c r="I17" s="113"/>
-      <c r="J17" s="114"/>
-      <c r="L17" s="146"/>
-      <c r="M17" s="137"/>
-      <c r="N17" s="137"/>
-      <c r="O17" s="137"/>
-      <c r="P17" s="137"/>
-      <c r="Q17" s="137"/>
-      <c r="R17" s="137"/>
-      <c r="S17" s="137"/>
-      <c r="T17" s="150"/>
-      <c r="U17" s="141" t="s">
-        <v>108</v>
-      </c>
-      <c r="IR17" s="138" t="s">
-        <v>149</v>
-      </c>
-      <c r="IS17" s="148"/>
-      <c r="IT17" s="33"/>
-      <c r="IU17" s="149" t="s">
-        <v>150</v>
-      </c>
-      <c r="IV17" s="149"/>
-      <c r="IW17" s="149"/>
-      <c r="IX17" s="149"/>
-      <c r="IY17" s="149"/>
+      <c r="F17" s="137"/>
+      <c r="G17" s="94"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="116"/>
+      <c r="J17" s="138"/>
+      <c r="L17" s="149"/>
+      <c r="M17" s="140"/>
+      <c r="N17" s="140"/>
+      <c r="O17" s="140"/>
+      <c r="P17" s="140"/>
+      <c r="Q17" s="140"/>
+      <c r="R17" s="140"/>
+      <c r="S17" s="140"/>
+      <c r="T17" s="153"/>
+      <c r="U17" s="144" t="s">
+        <v>106</v>
+      </c>
+      <c r="IR17" s="141" t="s">
+        <v>147</v>
+      </c>
+      <c r="IS17" s="151"/>
+      <c r="IT17" s="35"/>
+      <c r="IU17" s="152" t="s">
+        <v>148</v>
+      </c>
+      <c r="IV17" s="152"/>
+      <c r="IW17" s="152"/>
+      <c r="IX17" s="152"/>
+      <c r="IY17" s="152"/>
     </row>
     <row r="18" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="104" t="n">
+      <c r="A18" s="107" t="n">
         <f aca="false">A17+1</f>
         <v>14</v>
       </c>
-      <c r="B18" s="91"/>
-      <c r="C18" s="92"/>
-      <c r="D18" s="92"/>
-      <c r="E18" s="113" t="n">
+      <c r="B18" s="94"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="116" t="n">
         <f aca="false">PRODUCT(C18:D18)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="135"/>
-      <c r="G18" s="91"/>
-      <c r="H18" s="92"/>
-      <c r="I18" s="113"/>
-      <c r="J18" s="114"/>
-      <c r="L18" s="146"/>
-      <c r="M18" s="137"/>
-      <c r="N18" s="137"/>
-      <c r="O18" s="137"/>
-      <c r="P18" s="137"/>
-      <c r="Q18" s="137"/>
-      <c r="R18" s="137"/>
-      <c r="S18" s="137"/>
-      <c r="T18" s="151"/>
-      <c r="U18" s="120" t="s">
-        <v>151</v>
-      </c>
-      <c r="IR18" s="138" t="s">
-        <v>152</v>
-      </c>
-      <c r="IS18" s="148"/>
-      <c r="IT18" s="33"/>
-      <c r="IU18" s="149" t="s">
+      <c r="F18" s="137"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="95"/>
+      <c r="I18" s="116"/>
+      <c r="J18" s="138"/>
+      <c r="L18" s="149"/>
+      <c r="M18" s="140"/>
+      <c r="N18" s="140"/>
+      <c r="O18" s="140"/>
+      <c r="P18" s="140"/>
+      <c r="Q18" s="140"/>
+      <c r="R18" s="140"/>
+      <c r="S18" s="140"/>
+      <c r="T18" s="154"/>
+      <c r="U18" s="122" t="s">
+        <v>149</v>
+      </c>
+      <c r="IR18" s="141" t="s">
         <v>150</v>
       </c>
-      <c r="IV18" s="149"/>
-      <c r="IW18" s="149"/>
-      <c r="IX18" s="149"/>
-      <c r="IY18" s="149"/>
+      <c r="IS18" s="151"/>
+      <c r="IT18" s="35"/>
+      <c r="IU18" s="152" t="s">
+        <v>148</v>
+      </c>
+      <c r="IV18" s="152"/>
+      <c r="IW18" s="152"/>
+      <c r="IX18" s="152"/>
+      <c r="IY18" s="152"/>
     </row>
     <row r="19" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="104" t="n">
+      <c r="A19" s="107" t="n">
         <f aca="false">A18+1</f>
         <v>15</v>
       </c>
-      <c r="B19" s="91"/>
-      <c r="C19" s="92"/>
-      <c r="D19" s="92"/>
-      <c r="E19" s="113" t="n">
+      <c r="B19" s="94"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="116" t="n">
         <f aca="false">PRODUCT(C19:D19)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="135"/>
-      <c r="G19" s="91"/>
-      <c r="H19" s="92"/>
-      <c r="I19" s="113"/>
-      <c r="J19" s="114"/>
-      <c r="L19" s="146"/>
-      <c r="M19" s="137"/>
-      <c r="N19" s="137"/>
-      <c r="O19" s="137"/>
-      <c r="P19" s="137"/>
-      <c r="Q19" s="137"/>
-      <c r="R19" s="137"/>
-      <c r="S19" s="137"/>
-      <c r="T19" s="152"/>
-      <c r="U19" s="120" t="s">
-        <v>153</v>
-      </c>
-      <c r="IR19" s="153"/>
-      <c r="IS19" s="77"/>
-      <c r="IT19" s="154"/>
-      <c r="IU19" s="154"/>
-      <c r="IV19" s="154"/>
-      <c r="IW19" s="154"/>
-      <c r="IX19" s="154"/>
-      <c r="IY19" s="155"/>
+      <c r="F19" s="137"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="95"/>
+      <c r="I19" s="116"/>
+      <c r="J19" s="138"/>
+      <c r="L19" s="149"/>
+      <c r="M19" s="140"/>
+      <c r="N19" s="140"/>
+      <c r="O19" s="140"/>
+      <c r="P19" s="140"/>
+      <c r="Q19" s="140"/>
+      <c r="R19" s="140"/>
+      <c r="S19" s="140"/>
+      <c r="T19" s="155"/>
+      <c r="U19" s="122" t="s">
+        <v>151</v>
+      </c>
+      <c r="IR19" s="156"/>
+      <c r="IS19" s="80"/>
+      <c r="IT19" s="157"/>
+      <c r="IU19" s="157"/>
+      <c r="IV19" s="157"/>
+      <c r="IW19" s="157"/>
+      <c r="IX19" s="157"/>
+      <c r="IY19" s="158"/>
     </row>
     <row r="20" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="104" t="n">
+      <c r="A20" s="107" t="n">
         <f aca="false">A19+1</f>
         <v>16</v>
       </c>
-      <c r="B20" s="91"/>
-      <c r="C20" s="92"/>
-      <c r="D20" s="92"/>
-      <c r="E20" s="113" t="n">
+      <c r="B20" s="94"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="116" t="n">
         <f aca="false">PRODUCT(C20:D20)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="135"/>
-      <c r="G20" s="91"/>
-      <c r="H20" s="92"/>
-      <c r="I20" s="113"/>
-      <c r="J20" s="114"/>
-      <c r="L20" s="146"/>
-      <c r="M20" s="137"/>
-      <c r="N20" s="137"/>
-      <c r="O20" s="137"/>
-      <c r="P20" s="137"/>
-      <c r="Q20" s="137"/>
-      <c r="R20" s="137"/>
-      <c r="S20" s="137"/>
-      <c r="T20" s="156"/>
-      <c r="U20" s="157" t="s">
-        <v>154</v>
+      <c r="F20" s="137"/>
+      <c r="G20" s="94"/>
+      <c r="H20" s="95"/>
+      <c r="I20" s="116"/>
+      <c r="J20" s="138"/>
+      <c r="L20" s="149"/>
+      <c r="M20" s="140"/>
+      <c r="N20" s="140"/>
+      <c r="O20" s="140"/>
+      <c r="P20" s="140"/>
+      <c r="Q20" s="140"/>
+      <c r="R20" s="140"/>
+      <c r="S20" s="140"/>
+      <c r="T20" s="159"/>
+      <c r="U20" s="160" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambios plan de proyecto
</commit_message>
<xml_diff>
--- a/Proyectos/ControlDeGastos/02. Planeación/ControlDeGastos-PlanProyecto.xlsx
+++ b/Proyectos/ControlDeGastos/02. Planeación/ControlDeGastos-PlanProyecto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Generales" sheetId="1" state="visible" r:id="rId2"/>
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="156">
   <si>
     <t>Plan de Proyecto</t>
   </si>
@@ -425,6 +425,15 @@
   </si>
   <si>
     <t>Dar a conocer la finalización del proyecto en curso</t>
+  </si>
+  <si>
+    <t>Rene pulido</t>
+  </si>
+  <si>
+    <t>Notificar la finalización del proyecto al cliente</t>
+  </si>
+  <si>
+    <t>una vez por proyecto al finalizar proyecto</t>
   </si>
   <si>
     <t>Recursos Materiales</t>
@@ -2086,15 +2095,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1467000</xdr:colOff>
+      <xdr:colOff>1494000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3963960</xdr:colOff>
+      <xdr:colOff>3990600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>61920</xdr:rowOff>
+      <xdr:rowOff>61560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2107,8 +2116,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4248720" y="1080"/>
-          <a:ext cx="2496960" cy="822600"/>
+          <a:off x="4275720" y="1080"/>
+          <a:ext cx="2496600" cy="822240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2128,15 +2137,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>486000</xdr:colOff>
+      <xdr:colOff>513000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>136800</xdr:rowOff>
+      <xdr:rowOff>127800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>486360</xdr:colOff>
+      <xdr:colOff>513360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>128160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2145,7 +2154,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8297640" y="993960"/>
+          <a:off x="8324640" y="984960"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2171,15 +2180,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>981000</xdr:colOff>
+      <xdr:colOff>1008000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>136080</xdr:rowOff>
+      <xdr:rowOff>127080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>158760</xdr:colOff>
+      <xdr:colOff>185400</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>136440</xdr:rowOff>
+      <xdr:rowOff>127440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2188,8 +2197,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5045400" y="993240"/>
-          <a:ext cx="6348960" cy="360"/>
+          <a:off x="5072400" y="984240"/>
+          <a:ext cx="6348600" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2211,15 +2220,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>486000</xdr:colOff>
+      <xdr:colOff>513000</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>263880</xdr:rowOff>
+      <xdr:rowOff>254880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>486360</xdr:colOff>
+      <xdr:colOff>513360</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>264240</xdr:rowOff>
+      <xdr:rowOff>255240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2228,7 +2237,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8297640" y="5013000"/>
+          <a:off x="8324640" y="5004000"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2254,15 +2263,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>981000</xdr:colOff>
+      <xdr:colOff>1008000</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>263880</xdr:rowOff>
+      <xdr:rowOff>254880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>158760</xdr:colOff>
+      <xdr:colOff>185400</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>264240</xdr:rowOff>
+      <xdr:rowOff>255240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2271,8 +2280,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5045400" y="5013000"/>
-          <a:ext cx="6348960" cy="360"/>
+          <a:off x="5072400" y="5004000"/>
+          <a:ext cx="6348600" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2294,15 +2303,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>135000</xdr:colOff>
+      <xdr:colOff>162000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>135360</xdr:colOff>
+      <xdr:colOff>162360</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>851760</xdr:rowOff>
+      <xdr:rowOff>842400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2315,8 +2324,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12386520" y="29160"/>
-          <a:ext cx="360" cy="822600"/>
+          <a:off x="12413520" y="20160"/>
+          <a:ext cx="360" cy="822240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2336,15 +2345,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>628560</xdr:colOff>
+      <xdr:colOff>655560</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>13320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1686960</xdr:colOff>
+      <xdr:colOff>1713600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>844920</xdr:rowOff>
+      <xdr:rowOff>835560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2357,8 +2366,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10282320" y="22320"/>
-          <a:ext cx="2976840" cy="822600"/>
+          <a:off x="10309320" y="13320"/>
+          <a:ext cx="2976480" cy="822240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2378,15 +2387,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>800280</xdr:colOff>
+      <xdr:colOff>827280</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2173320</xdr:colOff>
+      <xdr:colOff>2199960</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>822600</xdr:rowOff>
+      <xdr:rowOff>822240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2399,8 +2408,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8276040" y="0"/>
-          <a:ext cx="2871720" cy="822600"/>
+          <a:off x="8303040" y="0"/>
+          <a:ext cx="2871360" cy="822240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2420,15 +2429,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1713600</xdr:colOff>
+      <xdr:colOff>1740600</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1888200</xdr:colOff>
+      <xdr:colOff>1914840</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>822600</xdr:rowOff>
+      <xdr:rowOff>822240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2441,8 +2450,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15088320" y="0"/>
-          <a:ext cx="3273480" cy="822600"/>
+          <a:off x="15115320" y="0"/>
+          <a:ext cx="3273120" cy="822240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2464,7 +2473,7 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -3111,8 +3120,8 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3263,12 +3272,22 @@
       <c r="G7" s="57"/>
       <c r="L7" s="58"/>
     </row>
-    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="54"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
+    <row r="8" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="55" t="s">
+        <v>83</v>
+      </c>
       <c r="G8" s="57"/>
       <c r="L8" s="58"/>
     </row>
@@ -3461,7 +3480,7 @@
     <row r="1" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="59" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B2" s="60"/>
       <c r="C2" s="60"/>
@@ -3472,33 +3491,33 @@
     </row>
     <row r="3" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="61" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B3" s="62" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C3" s="62" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D3" s="62" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E3" s="62" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F3" s="62" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G3" s="63" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="64" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C4" s="65"/>
       <c r="D4" s="65" t="n">
@@ -3512,15 +3531,15 @@
       </c>
       <c r="G4" s="67"/>
       <c r="J4" s="68" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="64" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C5" s="65"/>
       <c r="D5" s="65" t="n">
@@ -3534,15 +3553,15 @@
       </c>
       <c r="G5" s="67"/>
       <c r="J5" s="68" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="64" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C6" s="65"/>
       <c r="D6" s="65" t="n">
@@ -3556,15 +3575,15 @@
       </c>
       <c r="G6" s="67"/>
       <c r="J6" s="68" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="65" t="s">
         <v>96</v>
-      </c>
-      <c r="B7" s="65" t="s">
-        <v>93</v>
       </c>
       <c r="C7" s="65"/>
       <c r="D7" s="65" t="n">
@@ -3581,10 +3600,10 @@
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="64" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C8" s="65"/>
       <c r="D8" s="65" t="n">
@@ -3731,7 +3750,7 @@
       <c r="I2" s="71"/>
       <c r="J2" s="73"/>
       <c r="IQ2" s="74" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="IR2" s="74"/>
       <c r="IS2" s="74"/>
@@ -3745,7 +3764,7 @@
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="75" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B3" s="76"/>
       <c r="C3" s="77"/>
@@ -3760,45 +3779,45 @@
       <c r="M3" s="79"/>
       <c r="R3" s="80"/>
       <c r="AD3" s="81" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="AE3" s="81" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="82" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B4" s="82" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C4" s="83" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D4" s="83" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E4" s="83" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F4" s="83" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G4" s="83" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H4" s="83" t="s">
         <v>66</v>
       </c>
       <c r="I4" s="83" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="J4" s="83" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="L4" s="84" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="M4" s="85" t="n">
         <v>5</v>
@@ -3820,14 +3839,14 @@
       </c>
       <c r="S4" s="91"/>
       <c r="T4" s="92" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="U4" s="92"/>
       <c r="AD4" s="81" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="AE4" s="81" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="51.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3835,7 +3854,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="94" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C5" s="95" t="n">
         <v>3</v>
@@ -3848,16 +3867,16 @@
         <v>9</v>
       </c>
       <c r="F5" s="94" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G5" s="94" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="H5" s="95" t="s">
         <v>6</v>
       </c>
       <c r="I5" s="95" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="J5" s="96" t="s">
         <v>78</v>
@@ -3883,16 +3902,16 @@
       </c>
       <c r="S5" s="91"/>
       <c r="T5" s="100" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="U5" s="101" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="IR5" s="102" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="IS5" s="103" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="IT5" s="36" t="n">
         <v>0.9</v>
@@ -3924,7 +3943,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="94" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C6" s="95" t="n">
         <v>4</v>
@@ -3937,16 +3956,16 @@
         <v>12</v>
       </c>
       <c r="F6" s="94" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G6" s="94" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H6" s="95" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="95" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="J6" s="96" t="s">
         <v>78</v>
@@ -3975,11 +3994,11 @@
         <v>1</v>
       </c>
       <c r="U6" s="111" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="IR6" s="102"/>
       <c r="IS6" s="103" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="IT6" s="36" t="n">
         <v>0.7</v>
@@ -4011,7 +4030,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="94" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C7" s="95" t="n">
         <v>2</v>
@@ -4024,16 +4043,16 @@
         <v>8</v>
       </c>
       <c r="F7" s="94" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G7" s="94" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H7" s="95" t="s">
         <v>6</v>
       </c>
       <c r="I7" s="95" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="J7" s="96" t="s">
         <v>78</v>
@@ -4062,11 +4081,11 @@
         <v>2</v>
       </c>
       <c r="U7" s="122" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="IR7" s="102"/>
       <c r="IS7" s="103" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="IT7" s="36" t="n">
         <v>0.5</v>
@@ -4098,7 +4117,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="94" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C8" s="95" t="n">
         <v>5</v>
@@ -4111,16 +4130,16 @@
         <v>10</v>
       </c>
       <c r="F8" s="94" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="G8" s="94" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H8" s="95" t="s">
         <v>6</v>
       </c>
       <c r="I8" s="95" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="J8" s="96" t="s">
         <v>78</v>
@@ -4149,11 +4168,11 @@
         <v>3</v>
       </c>
       <c r="U8" s="122" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="IR8" s="102"/>
       <c r="IS8" s="103" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="IT8" s="36" t="n">
         <v>0.3</v>
@@ -4185,7 +4204,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="94" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C9" s="95" t="n">
         <v>3</v>
@@ -4198,16 +4217,16 @@
         <v>3</v>
       </c>
       <c r="F9" s="94" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="G9" s="94" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="H9" s="95" t="s">
         <v>6</v>
       </c>
       <c r="I9" s="95" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="J9" s="96" t="s">
         <v>78</v>
@@ -4234,11 +4253,11 @@
         <v>4</v>
       </c>
       <c r="U9" s="122" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="IR9" s="102"/>
       <c r="IS9" s="103" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="IT9" s="133" t="n">
         <v>0.1</v>
@@ -4284,7 +4303,7 @@
       <c r="L10" s="85"/>
       <c r="M10" s="129"/>
       <c r="N10" s="139" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="O10" s="139"/>
       <c r="P10" s="139"/>
@@ -4295,7 +4314,7 @@
         <v>5</v>
       </c>
       <c r="U10" s="122" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="IR10" s="141"/>
       <c r="IS10" s="79"/>
@@ -4342,28 +4361,28 @@
       <c r="R11" s="140"/>
       <c r="S11" s="140"/>
       <c r="T11" s="100" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="U11" s="144" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="IR11" s="141"/>
       <c r="IS11" s="79"/>
       <c r="IT11" s="79"/>
       <c r="IU11" s="103" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="IV11" s="103" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="IW11" s="103" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="IX11" s="103" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="IY11" s="145" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4395,13 +4414,13 @@
         <v>1</v>
       </c>
       <c r="U12" s="146" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="IR12" s="141"/>
       <c r="IS12" s="79"/>
       <c r="IT12" s="36"/>
       <c r="IU12" s="147" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="IV12" s="147"/>
       <c r="IW12" s="147"/>
@@ -4437,7 +4456,7 @@
         <v>2</v>
       </c>
       <c r="U13" s="111" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="IR13" s="141"/>
       <c r="IS13" s="79"/>
@@ -4477,7 +4496,7 @@
         <v>3</v>
       </c>
       <c r="U14" s="122" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="IR14" s="141"/>
       <c r="IS14" s="79"/>
@@ -4517,10 +4536,10 @@
         <v>4</v>
       </c>
       <c r="U15" s="122" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="IR15" s="150" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="IS15" s="150"/>
       <c r="IT15" s="35"/>
@@ -4559,15 +4578,15 @@
         <v>5</v>
       </c>
       <c r="U16" s="146" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="IR16" s="141" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="IS16" s="151"/>
       <c r="IT16" s="35"/>
       <c r="IU16" s="152" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="IV16" s="152"/>
       <c r="IW16" s="152"/>
@@ -4601,15 +4620,15 @@
       <c r="S17" s="140"/>
       <c r="T17" s="153"/>
       <c r="U17" s="144" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="IR17" s="141" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="IS17" s="151"/>
       <c r="IT17" s="35"/>
       <c r="IU17" s="152" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="IV17" s="152"/>
       <c r="IW17" s="152"/>
@@ -4643,15 +4662,15 @@
       <c r="S18" s="140"/>
       <c r="T18" s="154"/>
       <c r="U18" s="122" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="IR18" s="141" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="IS18" s="151"/>
       <c r="IT18" s="35"/>
       <c r="IU18" s="152" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="IV18" s="152"/>
       <c r="IW18" s="152"/>
@@ -4685,7 +4704,7 @@
       <c r="S19" s="140"/>
       <c r="T19" s="155"/>
       <c r="U19" s="122" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="IR19" s="156"/>
       <c r="IS19" s="80"/>
@@ -4723,7 +4742,7 @@
       <c r="S20" s="140"/>
       <c r="T20" s="159"/>
       <c r="U20" s="160" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>